<commit_message>
Categorizacion de tipo de preguntas para diccionario demo
</commit_message>
<xml_diff>
--- a/vignettes/Manual-diccionario/diccionario_ejemp_gen.xlsx
+++ b/vignettes/Manual-diccionario/diccionario_ejemp_gen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\GitHub\encuestar\Documentacion\diccionario\insumos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\al-jo\Git\encuestar\vignettes\Manual-diccionario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BC8309-C94C-4458-A8A8-F9DF3C26C478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD51EA7A-FC16-4302-AFDA-0931B4F43152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
   <si>
     <t>bloque</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t xml:space="preserve">¿Por cuál partido o candidato votó usted para Gobernador de Sonora 2024? </t>
+  </si>
+  <si>
+    <t>tipo_metodo</t>
+  </si>
+  <si>
+    <t>piramide</t>
+  </si>
+  <si>
+    <t>abierta</t>
+  </si>
+  <si>
+    <t>categorica</t>
   </si>
 </sst>
 </file>
@@ -527,22 +539,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC726119-F10F-4E4C-8405-3FF2B301E575}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.21875" customWidth="1"/>
-    <col min="2" max="2" width="97.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="97.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,8 +575,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -577,8 +594,11 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -595,8 +615,11 @@
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -611,8 +634,11 @@
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -625,8 +651,11 @@
       <c r="D5" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>31</v>
       </c>
@@ -642,8 +671,11 @@
       <c r="F6" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>31</v>
       </c>
@@ -659,8 +691,11 @@
       <c r="F7" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>31</v>
       </c>
@@ -675,8 +710,11 @@
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>35</v>
       </c>
@@ -693,8 +731,11 @@
       <c r="F9" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>35</v>
       </c>
@@ -709,8 +750,11 @@
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
@@ -727,8 +771,11 @@
       <c r="F11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>39</v>
       </c>
@@ -743,8 +790,11 @@
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>42</v>
       </c>
@@ -761,8 +811,11 @@
       <c r="F13" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>42</v>
       </c>
@@ -777,8 +830,11 @@
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>45</v>
       </c>
@@ -797,8 +853,11 @@
       <c r="F15" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>45</v>
       </c>
@@ -817,8 +876,11 @@
       <c r="F16" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>45</v>
       </c>
@@ -837,8 +899,11 @@
       <c r="F17" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>45</v>
       </c>
@@ -857,8 +922,11 @@
       <c r="F18" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>45</v>
       </c>
@@ -875,8 +943,11 @@
         <v>52</v>
       </c>
       <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>45</v>
       </c>
@@ -893,8 +964,11 @@
         <v>51</v>
       </c>
       <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>45</v>
       </c>
@@ -912,6 +986,9 @@
       </c>
       <c r="F21" s="10" t="s">
         <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>